<commit_message>
updated documenation for clarity
</commit_message>
<xml_diff>
--- a/documentation/config_explained.xlsx
+++ b/documentation/config_explained.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="913" uniqueCount="499">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="914" uniqueCount="500">
   <si>
     <t xml:space="preserve">top-level parameters</t>
   </si>
@@ -305,6 +305,9 @@
   </si>
   <si>
     <t xml:space="preserve">sequence of reverse primer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Direction : 5’ to 3’ of the primer itself</t>
   </si>
   <si>
     <t xml:space="preserve">    name</t>
@@ -1609,7 +1612,7 @@
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.00E+00"/>
-    <numFmt numFmtId="166" formatCode="D\-MMM"/>
+    <numFmt numFmtId="166" formatCode="d\-mmm"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -1760,12 +1763,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -1835,21 +1838,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:H181"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="101" zoomScaleNormal="101" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C106" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="E6" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A106" activeCellId="0" sqref="A106"/>
-      <selection pane="bottomRight" activeCell="C118" activeCellId="0" sqref="C118"/>
+      <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="bottomLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+      <selection pane="bottomRight" activeCell="H23" activeCellId="0" sqref="H23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.6015625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.52"/>
@@ -1859,7 +1862,6 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="40.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="48.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="10.61"/>
   </cols>
   <sheetData>
     <row r="1" s="4" customFormat="true" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2374,7 +2376,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="6"/>
       <c r="B23" s="6"/>
       <c r="C23" s="0" t="s">
@@ -2392,24 +2394,27 @@
       <c r="G23" s="1" t="s">
         <v>93</v>
       </c>
+      <c r="H23" s="1" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="6"/>
       <c r="B24" s="6"/>
       <c r="C24" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="F24" s="0" t="s">
         <v>92</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="H24" s="1" t="s">
         <v>86</v>
@@ -2417,176 +2422,176 @@
     </row>
     <row r="25" customFormat="false" ht="68" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>38</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="F26" s="0" t="s">
         <v>92</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="6" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="F27" s="0" t="s">
         <v>92</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="6"/>
       <c r="B28" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D28" s="0" t="n">
         <v>10</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F28" s="0" t="s">
         <v>92</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="6"/>
       <c r="B29" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D29" s="0" t="n">
         <v>2</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="F29" s="0" t="s">
         <v>92</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="6"/>
       <c r="B30" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="F30" s="0" t="s">
         <v>92</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="6"/>
       <c r="B31" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D31" s="0" t="n">
         <v>0.2</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F31" s="0" t="s">
         <v>92</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="6"/>
       <c r="B32" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="F32" s="0" t="s">
         <v>92</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="6"/>
       <c r="B33" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D33" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="F33" s="0" t="s">
         <v>92</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="102" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="6" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B34" s="0" t="s">
         <v>9</v>
@@ -2601,451 +2606,451 @@
         <v>10</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G34" s="1" t="s">
         <v>10</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="6"/>
       <c r="B35" s="6" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="6"/>
       <c r="B36" s="6"/>
       <c r="C36" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D36" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="6"/>
       <c r="B37" s="6"/>
       <c r="C37" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D37" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="6"/>
       <c r="B38" s="7" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="F38" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="6"/>
       <c r="B39" s="7"/>
       <c r="C39" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D39" s="0" t="n">
         <v>2</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="F39" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="6"/>
       <c r="B40" s="7"/>
       <c r="C40" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D40" s="0" t="n">
         <v>2</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="F40" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="6"/>
       <c r="B41" s="6" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="F41" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="6"/>
       <c r="B42" s="6"/>
       <c r="C42" s="0" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D42" s="0" t="n">
         <v>2</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="F42" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="68" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="6"/>
       <c r="B43" s="6"/>
       <c r="C43" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D43" s="0" t="n">
         <v>2</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="F43" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="6"/>
       <c r="B44" s="6" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F44" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="6"/>
       <c r="B45" s="6"/>
       <c r="C45" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D45" s="0" t="n">
         <v>20</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="F45" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="6"/>
       <c r="B46" s="6"/>
       <c r="C46" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D46" s="0" t="n">
         <v>20</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="F46" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="6"/>
       <c r="B47" s="6" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F47" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="6"/>
       <c r="B48" s="6"/>
       <c r="C48" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D48" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="F48" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="6"/>
       <c r="B49" s="6"/>
       <c r="C49" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D49" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="F49" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="6"/>
       <c r="B50" s="6" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="F50" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="6"/>
       <c r="B51" s="6"/>
       <c r="C51" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D51" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="F51" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="6"/>
       <c r="B52" s="6"/>
       <c r="C52" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D52" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="F52" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="H52" s="1" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="6"/>
       <c r="B53" s="6" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="F53" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="H53" s="1" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="6"/>
       <c r="B54" s="6"/>
       <c r="C54" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D54" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="F54" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="H54" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="6"/>
       <c r="B55" s="6"/>
       <c r="C55" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D55" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="F55" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="G55" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="H55" s="5" t="s">
         <v>182</v>
-      </c>
-      <c r="H55" s="5" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="6"/>
       <c r="B56" s="8" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="E56" s="1" t="s">
         <v>38</v>
       </c>
       <c r="F56" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="H56" s="1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="D57" s="0" t="n">
         <v>100</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="F57" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="G57" s="1" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="H57" s="1" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="6" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="F58" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="6"/>
       <c r="B59" s="0" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="D59" s="5" t="s">
         <v>37</v>
@@ -3054,1675 +3059,1675 @@
         <v>38</v>
       </c>
       <c r="F59" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="6"/>
       <c r="B60" s="0" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="D60" s="0" t="n">
         <v>50000</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="F60" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="6"/>
       <c r="B61" s="0" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="D61" s="5" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="E61" s="1" t="s">
         <v>38</v>
       </c>
       <c r="F61" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="H61" s="1" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="6"/>
       <c r="B62" s="0" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="D62" s="0" t="n">
         <v>123</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="F62" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="F63" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="H63" s="1" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="9"/>
       <c r="B64" s="0" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="D64" s="0" t="n">
         <v>16</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="F64" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="G64" s="1" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="H64" s="1" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="68" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="9"/>
       <c r="B65" s="0" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="D65" s="0" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="F65" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="G65" s="1" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="H65" s="1" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="136" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="9"/>
       <c r="B66" s="0" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="D66" s="0" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="F66" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="G66" s="1" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="H66" s="1" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="9"/>
       <c r="B67" s="0" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="D67" s="10" t="n">
         <v>1E-040</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="F67" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="G67" s="1" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="H67" s="1" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="9"/>
       <c r="B68" s="0" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="D68" s="0" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="F68" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="G68" s="1" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="H68" s="1" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="9"/>
       <c r="B69" s="0" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="D69" s="10" t="n">
         <v>0.0001</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="F69" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="G69" s="1" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="H69" s="1" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="9"/>
       <c r="B70" s="0" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="D70" s="10" t="n">
         <v>1E-040</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="F70" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="G70" s="1" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="H70" s="1" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="9"/>
       <c r="B71" s="0" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="D71" s="0" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="E71" s="1" t="s">
         <v>38</v>
       </c>
       <c r="F71" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="G71" s="1" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="H71" s="1" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="9"/>
       <c r="B72" s="0" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="D72" s="0" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="E72" s="1" t="s">
         <v>38</v>
       </c>
       <c r="F72" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="G72" s="1" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="H72" s="1" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="9"/>
       <c r="B73" s="0" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="D73" s="0" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="F73" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="G73" s="1" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="H73" s="1" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="9"/>
       <c r="B74" s="0" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="D74" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E74" s="1" t="s">
         <v>38</v>
       </c>
       <c r="F74" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="G74" s="1" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="H74" s="1" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="9"/>
       <c r="B75" s="0" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="D75" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E75" s="1" t="s">
         <v>38</v>
       </c>
       <c r="F75" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="G75" s="1" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="H75" s="1" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="9"/>
       <c r="B76" s="0" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="D76" s="0" t="n">
         <v>0.42</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="F76" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="G76" s="1" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="H76" s="1" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="9"/>
       <c r="B77" s="0" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="D77" s="0" t="n">
         <v>4</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="F77" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="G77" s="1" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="H77" s="1" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="9"/>
       <c r="B78" s="0" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="D78" s="0" t="n">
         <v>-5</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="F78" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="G78" s="1" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="H78" s="1" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="9"/>
       <c r="B79" s="0" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="D79" s="0" t="n">
         <v>-8</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="F79" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="G79" s="1" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="H79" s="1" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="6" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="F80" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="H80" s="1" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="6"/>
       <c r="B81" s="0" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="D81" s="0" t="n">
         <v>12</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="F81" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="G81" s="1" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="H81" s="1" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="6"/>
       <c r="B82" s="0" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="D82" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="F82" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="G82" s="1" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="H82" s="1" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="68" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="6"/>
       <c r="B83" s="0" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="D83" s="0" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="E83" s="1" t="s">
         <v>38</v>
       </c>
       <c r="F83" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="G83" s="1" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="H83" s="1" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="6"/>
       <c r="B84" s="0" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="D84" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E84" s="1" t="s">
         <v>38</v>
       </c>
       <c r="F84" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="G84" s="1" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="H84" s="1" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="6" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="F85" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="H85" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="6"/>
       <c r="B86" s="0" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="D86" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E86" s="1" t="s">
         <v>38</v>
       </c>
       <c r="F86" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="G86" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="6"/>
       <c r="B87" s="0" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="D87" s="0" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="F87" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="G87" s="1" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="H87" s="1" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="6"/>
       <c r="B88" s="0" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="D88" s="0" t="n">
         <v>2</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="F88" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="G88" s="1" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="H88" s="1" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="6"/>
       <c r="B89" s="0" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="D89" s="0" t="n">
         <v>8</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="F89" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="G89" s="1" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="H89" s="1" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="6"/>
       <c r="B90" s="0" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="D90" s="0" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="E90" s="1" t="s">
         <v>38</v>
       </c>
       <c r="F90" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="G90" s="1" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="H90" s="1" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="6"/>
       <c r="B91" s="0" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="D91" s="0" t="n">
         <v>4</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="F91" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="G91" s="1" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="H91" s="1" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="6"/>
       <c r="B92" s="0" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="D92" s="0" t="n">
         <v>16</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="F92" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="G92" s="1" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="H92" s="1" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="6" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="F93" s="0" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="H93" s="1" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="6"/>
       <c r="B94" s="6" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="F94" s="0" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="H94" s="1" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="37.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="6"/>
       <c r="B95" s="6"/>
       <c r="C95" s="0" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="D95" s="0" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="E95" s="1" t="s">
         <v>38</v>
       </c>
       <c r="F95" s="0" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="G95" s="1" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="H95" s="1" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="6"/>
       <c r="B96" s="6"/>
       <c r="C96" s="0" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="D96" s="0" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="E96" s="1" t="s">
         <v>38</v>
       </c>
       <c r="F96" s="0" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="G96" s="1" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="H96" s="1" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="6"/>
       <c r="B97" s="6"/>
       <c r="C97" s="0" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="D97" s="0" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="F97" s="0" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="G97" s="1" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="H97" s="1" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="6"/>
       <c r="B98" s="6"/>
       <c r="C98" s="0" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="D98" s="0" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="F98" s="0" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="G98" s="1" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="H98" s="1" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="6"/>
       <c r="B99" s="6"/>
       <c r="C99" s="0" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="D99" s="0" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="F99" s="0" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="G99" s="1" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="H99" s="1" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="6"/>
       <c r="B100" s="6"/>
       <c r="C100" s="0" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="D100" s="0" t="s">
         <v>17</v>
       </c>
       <c r="F100" s="0" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="G100" s="1" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="H100" s="1" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="6"/>
       <c r="B101" s="6"/>
       <c r="C101" s="0" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="D101" s="0" t="n">
         <v>50</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="F101" s="0" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="G101" s="1" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="H101" s="1" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="6"/>
       <c r="B102" s="6"/>
       <c r="C102" s="0" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="D102" s="0" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="E102" s="1" t="s">
         <v>38</v>
       </c>
       <c r="F102" s="0" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="G102" s="1" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="H102" s="1" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="6"/>
       <c r="B103" s="6"/>
       <c r="C103" s="0" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="D103" s="0" t="n">
         <v>100</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="F103" s="0" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="G103" s="1" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="H103" s="1" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="6"/>
       <c r="B104" s="6"/>
       <c r="C104" s="11" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="D104" s="0" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="E104" s="1" t="s">
         <v>38</v>
       </c>
       <c r="F104" s="0" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="G104" s="1" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="H104" s="12" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="6"/>
       <c r="B105" s="6"/>
       <c r="C105" s="0" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="D105" s="0" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="F105" s="0" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="G105" s="1" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="H105" s="1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="6"/>
       <c r="B106" s="6" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="F106" s="0" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="H106" s="1" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="49.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="6"/>
       <c r="B107" s="6"/>
       <c r="C107" s="0" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="D107" s="0" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="F107" s="0" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="G107" s="1" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="H107" s="13" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="6"/>
       <c r="B108" s="6"/>
       <c r="C108" s="0" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="D108" s="0" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="E108" s="1" t="s">
         <v>38</v>
       </c>
       <c r="F108" s="0" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="G108" s="1" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="H108" s="1" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="6"/>
       <c r="B109" s="6"/>
       <c r="C109" s="0" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="D109" s="0" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="F109" s="0" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="G109" s="1" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="H109" s="1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="6"/>
       <c r="B110" s="6"/>
       <c r="C110" s="0" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="D110" s="0" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="F110" s="0" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="G110" s="1" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="6"/>
       <c r="B111" s="6"/>
       <c r="C111" s="0" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="D111" s="0" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="F111" s="0" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="G111" s="1" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="H111" s="1" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="6"/>
       <c r="B112" s="6"/>
       <c r="C112" s="0" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="D112" s="0" t="s">
         <v>17</v>
       </c>
       <c r="F112" s="0" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="G112" s="1" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="H112" s="1" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="6"/>
       <c r="B113" s="6"/>
       <c r="C113" s="0" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="D113" s="0" t="n">
         <v>60</v>
       </c>
       <c r="E113" s="1" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="F113" s="0" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="G113" s="1" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="H113" s="1" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="6"/>
       <c r="B114" s="6"/>
       <c r="C114" s="0" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D114" s="0" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="E114" s="1" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="F114" s="0" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="G114" s="1" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="H114" s="1" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="6"/>
       <c r="B115" s="6"/>
       <c r="C115" s="0" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="D115" s="0" t="n">
         <v>100</v>
       </c>
       <c r="E115" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="F115" s="0" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="G115" s="1" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="6"/>
       <c r="B116" s="6"/>
       <c r="C116" s="0" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="D116" s="0" t="n">
         <v>100</v>
       </c>
       <c r="E116" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="F116" s="0" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="G116" s="1" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="H116" s="1" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="6"/>
       <c r="B117" s="6"/>
       <c r="C117" s="11" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="D117" s="0" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="E117" s="1" t="s">
         <v>38</v>
       </c>
       <c r="F117" s="0" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="G117" s="1" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="H117" s="1" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="25.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="6"/>
       <c r="B118" s="6"/>
       <c r="C118" s="0" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="D118" s="0" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="F118" s="0" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="G118" s="1" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="H118" s="1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="6"/>
       <c r="B119" s="6" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="F119" s="0" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="H119" s="1" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="68" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="6"/>
       <c r="B120" s="6"/>
       <c r="C120" s="0" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="D120" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E120" s="1" t="s">
         <v>38</v>
       </c>
       <c r="F120" s="0" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="G120" s="1" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="H120" s="1" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="6"/>
       <c r="B121" s="6"/>
       <c r="C121" s="0" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="D121" s="0" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="E121" s="1" t="s">
         <v>38</v>
       </c>
       <c r="F121" s="0" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="G121" s="1" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="H121" s="1" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="6"/>
       <c r="B122" s="6"/>
       <c r="C122" s="0" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="D122" s="0" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="F122" s="0" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="G122" s="1" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="H122" s="1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="6"/>
       <c r="B123" s="6"/>
       <c r="C123" s="0" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="D123" s="0" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="F123" s="0" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="G123" s="1" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="H123" s="1" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="6"/>
       <c r="B124" s="6"/>
       <c r="C124" s="0" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="D124" s="0" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="F124" s="0" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="G124" s="1" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="H124" s="1" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="6"/>
       <c r="B125" s="6"/>
       <c r="C125" s="0" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="D125" s="0" t="s">
         <v>17</v>
       </c>
       <c r="F125" s="0" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="G125" s="1" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="H125" s="1" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="6"/>
       <c r="B126" s="6"/>
       <c r="C126" s="0" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="D126" s="0" t="n">
         <v>60</v>
       </c>
       <c r="E126" s="1" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="F126" s="0" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="G126" s="1" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="6" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="F127" s="0" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="25.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="6"/>
       <c r="B128" s="0" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="D128" s="5" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="E128" s="1" t="s">
         <v>38</v>
       </c>
       <c r="F128" s="0" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="G128" s="1" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="H128" s="1" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="6"/>
       <c r="B129" s="0" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="D129" s="0" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="F129" s="0" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="G129" s="1" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="6"/>
       <c r="B130" s="0" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="D130" s="0" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="F130" s="0" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="G130" s="1" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="6"/>
       <c r="B131" s="0" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="D131" s="0" t="n">
         <v>0.01</v>
       </c>
       <c r="F131" s="0" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="G131" s="1" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="6"/>
       <c r="B132" s="0" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="D132" s="0" t="s">
         <v>17</v>
       </c>
       <c r="E132" s="1" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="F132" s="0" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="G132" s="1" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="H132" s="1" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="6"/>
       <c r="B133" s="0" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="D133" s="0" t="n">
         <v>10</v>
       </c>
       <c r="E133" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="F133" s="0" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="G133" s="1" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="6"/>
       <c r="B134" s="0" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="D134" s="5" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="E134" s="1" t="s">
         <v>38</v>
       </c>
       <c r="F134" s="0" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="G134" s="1" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="H134" s="1" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="6"/>
       <c r="B135" s="0" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="D135" s="5" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="E135" s="1" t="s">
         <v>38</v>
       </c>
       <c r="F135" s="0" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="G135" s="1" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="6"/>
       <c r="B136" s="0" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="D136" s="5" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="F136" s="0" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="G136" s="1" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="H136" s="1" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="6"/>
       <c r="B137" s="0" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="D137" s="0" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="F137" s="0" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="G137" s="1" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="H137" s="1" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="6"/>
       <c r="B138" s="0" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="D138" s="0" t="n">
         <v>1E-005</v>
       </c>
       <c r="E138" s="1" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="F138" s="0" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="G138" s="1" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="6"/>
       <c r="B139" s="0" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="D139" s="0" t="n">
         <v>100</v>
       </c>
       <c r="E139" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="F139" s="0" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="G139" s="1" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="6"/>
       <c r="B140" s="0" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="D140" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E140" s="1" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="F140" s="0" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="G140" s="1" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="H140" s="1" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="6"/>
       <c r="B141" s="0" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D141" s="0" t="n">
         <v>3</v>
       </c>
       <c r="E141" s="1" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="F141" s="0" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="G141" s="1" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="H141" s="1" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="6"/>
       <c r="B142" s="0" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="D142" s="0" t="n">
         <v>80</v>
       </c>
       <c r="E142" s="1" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="F142" s="0" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="G142" s="1" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="6"/>
       <c r="B143" s="0" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="D143" s="5" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="E143" s="1" t="s">
         <v>38</v>
       </c>
       <c r="F143" s="0" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="G143" s="1" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="6"/>
       <c r="B144" s="0" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="D144" s="0" t="n">
         <v>99</v>
       </c>
       <c r="E144" s="1" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="F144" s="0" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="G144" s="1" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="6" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="F145" s="0" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="H145" s="1" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="6"/>
       <c r="B146" s="0" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="D146" s="0" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="E146" s="1" t="s">
         <v>38</v>
       </c>
       <c r="F146" s="0" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="G146" s="1" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="H146" s="1" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="6"/>
       <c r="B147" s="0" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="D147" s="0" t="n">
         <v>1</v>
@@ -4731,129 +4736,129 @@
         <v>43922</v>
       </c>
       <c r="F147" s="0" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="G147" s="1" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="H147" s="1" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="6"/>
       <c r="B148" s="0" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="D148" s="0" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="E148" s="1" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="F148" s="0" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="G148" s="1" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="6"/>
       <c r="B149" s="0" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="D149" s="0" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="E149" s="1" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="F149" s="0" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="G149" s="1" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="H149" s="1" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="6"/>
       <c r="B150" s="0" t="s">
+        <v>425</v>
+      </c>
+      <c r="D150" s="0" t="s">
+        <v>426</v>
+      </c>
+      <c r="E150" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="F150" s="0" t="s">
+        <v>287</v>
+      </c>
+      <c r="G150" s="1" t="s">
+        <v>428</v>
+      </c>
+      <c r="H150" s="1" t="s">
         <v>424</v>
-      </c>
-      <c r="D150" s="0" t="s">
-        <v>425</v>
-      </c>
-      <c r="E150" s="1" t="s">
-        <v>426</v>
-      </c>
-      <c r="F150" s="0" t="s">
-        <v>286</v>
-      </c>
-      <c r="G150" s="1" t="s">
-        <v>427</v>
-      </c>
-      <c r="H150" s="1" t="s">
-        <v>423</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="6"/>
       <c r="B151" s="0" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="D151" s="10" t="n">
         <v>1E-005</v>
       </c>
       <c r="E151" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F151" s="0" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="G151" s="1" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="6" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="F152" s="0" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="H152" s="1" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="6"/>
       <c r="B153" s="0" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="D153" s="5" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="E153" s="1" t="s">
         <v>38</v>
       </c>
       <c r="F153" s="0" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="G153" s="1" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="H153" s="1" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="6"/>
       <c r="B154" s="0" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="D154" s="5" t="s">
         <v>37</v>
@@ -4862,126 +4867,126 @@
         <v>38</v>
       </c>
       <c r="F154" s="0" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="G154" s="1" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="H154" s="1" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="6" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="F155" s="0" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="H155" s="1" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="6"/>
       <c r="B156" s="0" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="D156" s="5" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="E156" s="1" t="s">
         <v>38</v>
       </c>
       <c r="F156" s="0" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="G156" s="1" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="6"/>
       <c r="B157" s="0" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="D157" s="0" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="E157" s="1" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="F157" s="0" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="G157" s="1" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="H157" s="1" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="6"/>
       <c r="B158" s="0" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="D158" s="0" t="n">
         <v>1</v>
       </c>
       <c r="F158" s="0" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="G158" s="1" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="H158" s="1" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="6"/>
       <c r="B159" s="0" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="D159" s="0" t="n">
         <v>10000</v>
       </c>
       <c r="F159" s="0" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="G159" s="1" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="H159" s="1" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="7" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="F160" s="0" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="H160" s="1" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="7"/>
       <c r="B161" s="7" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="F161" s="0" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="7"/>
       <c r="B162" s="7"/>
       <c r="C162" s="0" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="D162" s="5" t="s">
         <v>37</v>
@@ -4990,67 +4995,67 @@
         <v>38</v>
       </c>
       <c r="F162" s="0" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="7"/>
       <c r="B163" s="7"/>
       <c r="C163" s="0" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="D163" s="0" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="E163" s="1" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="F163" s="0" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="G163" s="1" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="H163" s="1" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="7"/>
       <c r="B164" s="7"/>
       <c r="C164" s="0" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="D164" s="0" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="F164" s="0" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="G164" s="1" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="H164" s="1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="7"/>
       <c r="B165" s="6" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="F165" s="0" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="H165" s="1" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="7"/>
       <c r="B166" s="6"/>
       <c r="C166" s="0" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="D166" s="5" t="s">
         <v>37</v>
@@ -5059,70 +5064,70 @@
         <v>38</v>
       </c>
       <c r="F166" s="0" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="G166" s="1" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="7"/>
       <c r="B167" s="6"/>
       <c r="C167" s="0" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="D167" s="0" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="F167" s="0" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="G167" s="1" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="H167" s="1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="7"/>
       <c r="B168" s="6"/>
       <c r="C168" s="0" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="D168" s="0" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="E168" s="1" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="F168" s="0" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="G168" s="1" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="H168" s="1" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="7"/>
       <c r="B169" s="7" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="F169" s="0" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="H169" s="1" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="25.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="7"/>
       <c r="B170" s="7"/>
       <c r="C170" s="0" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="D170" s="5" t="s">
         <v>37</v>
@@ -5131,39 +5136,39 @@
         <v>38</v>
       </c>
       <c r="F170" s="0" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="G170" s="1" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="H170" s="1" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="7"/>
       <c r="B171" s="7"/>
       <c r="C171" s="0" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="D171" s="0" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="F171" s="0" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="G171" s="1" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="H171" s="1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="7"/>
       <c r="B172" s="7"/>
       <c r="C172" s="0" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="D172" s="5" t="s">
         <v>37</v>
@@ -5172,167 +5177,167 @@
         <v>38</v>
       </c>
       <c r="F172" s="0" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="G172" s="1" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="7"/>
       <c r="B173" s="7"/>
       <c r="C173" s="0" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="D173" s="0" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="F173" s="0" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="G173" s="1" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="7"/>
       <c r="B174" s="7"/>
       <c r="C174" s="0" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="D174" s="0" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="F174" s="0" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="G174" s="1" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="7"/>
       <c r="B175" s="7"/>
       <c r="C175" s="0" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="D175" s="0" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="E175" s="1" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="F175" s="0" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="G175" s="1" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="7"/>
       <c r="B176" s="7"/>
       <c r="C176" s="0" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="D176" s="5" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="E176" s="1" t="s">
         <v>38</v>
       </c>
       <c r="F176" s="0" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="G176" s="1" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="H176" s="1" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="7"/>
       <c r="B177" s="7"/>
       <c r="C177" s="0" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="D177" s="0" t="n">
         <v>0.97</v>
       </c>
       <c r="E177" s="1" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="F177" s="0" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="G177" s="1" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="7"/>
       <c r="B178" s="6" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="E178" s="1" t="s">
         <v>38</v>
       </c>
       <c r="F178" s="0" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="7"/>
       <c r="B179" s="6"/>
       <c r="C179" s="0" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="D179" s="5" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="F179" s="0" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="G179" s="1" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="7"/>
       <c r="B180" s="6"/>
       <c r="C180" s="0" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="D180" s="0" t="s">
         <v>17</v>
       </c>
       <c r="F180" s="0" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="G180" s="1" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="H180" s="1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="7"/>
       <c r="B181" s="0" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="D181" s="5" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="E181" s="1" t="s">
         <v>38</v>
       </c>
       <c r="F181" s="0" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="G181" s="1" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
clarify primer_cutting/perc_mismatch is a fraction, not %
</commit_message>
<xml_diff>
--- a/documentation/config_explained.xlsx
+++ b/documentation/config_explained.xlsx
@@ -397,7 +397,7 @@
     <t xml:space="preserve">0-1</t>
   </si>
   <si>
-    <t xml:space="preserve">% mismatch between read and each primer</t>
+    <t xml:space="preserve">fraction (not really %) mismatch between read and each primer</t>
   </si>
   <si>
     <t xml:space="preserve">don't set this to 1</t>
@@ -1770,6 +1770,37 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <dxfs count="4">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFF9AE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="00FFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF000000"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFF685"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -1845,17 +1876,17 @@
   <dimension ref="A1:H181"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="101" zoomScaleNormal="101" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="E6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="F28" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="H23" activeCellId="0" sqref="H23"/>
+      <selection pane="topRight" activeCell="F1" activeCellId="0" sqref="F1"/>
+      <selection pane="bottomLeft" activeCell="A28" activeCellId="0" sqref="A28"/>
+      <selection pane="bottomRight" activeCell="G32" activeCellId="0" sqref="G32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6015625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.609375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="29.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="35.33"/>
@@ -2528,7 +2559,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="6"/>
       <c r="B31" s="0" t="s">
         <v>122</v>
@@ -5377,8 +5408,8 @@
     <hyperlink ref="H170" r:id="rId1" display="Predicts functional profiles based on 16s rRNA sequences (reference: 2020)"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>